<commit_message>
220707-v2 dout_sel has one time delay, to be remove _sel <= _sel_new
</commit_message>
<xml_diff>
--- a/非线性计算模块的状态表.xlsx
+++ b/非线性计算模块的状态表.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C585C652-51FC-4E5D-9C6B-277BDAB96C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D56D7D3-70DA-440E-B95E-3DF28341351E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="2123" windowWidth="9585" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3908" yWindow="3150" windowWidth="9585" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,20 +579,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1217,15 +1217,15 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="7" t="s">
         <v>25</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -1284,7 +1284,7 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="3"/>
       <c r="C7" s="7" t="s">
         <v>26</v>
@@ -1316,7 +1316,7 @@
       <c r="X7" s="3"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>24</v>
@@ -1349,7 +1349,7 @@
       <c r="X8" s="3"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7" t="s">
         <v>38</v>
@@ -1380,7 +1380,7 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1421,7 +1421,7 @@
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1462,9 +1462,9 @@
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1498,9 +1498,9 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A14" s="16"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="7" t="s">
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="Y15" s="5"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="12" t="s">
         <v>21</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="Y16" s="5"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="9" t="s">
         <v>22</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
@@ -1683,7 +1683,7 @@
       <c r="Y18" s="5"/>
     </row>
     <row r="19" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1717,7 +1717,7 @@
       <c r="Y19" s="8"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1751,7 +1751,7 @@
       <c r="Y20" s="5"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1782,7 +1782,7 @@
       <c r="Y21" s="5"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -1888,13 +1888,13 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1917,29 +1917,29 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:25" ht="27.75" x14ac:dyDescent="0.4">
@@ -1967,56 +1967,56 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="9"/>
     </row>
     <row r="33" spans="3:24" x14ac:dyDescent="0.4">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-      <c r="V33" s="14"/>
-      <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.4">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="8"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -2045,6 +2045,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A5:A22"/>
     <mergeCell ref="T33:V33"/>
     <mergeCell ref="W33:X33"/>
     <mergeCell ref="F34:J34"/>
@@ -2052,13 +2059,6 @@
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="F33:J33"/>
     <mergeCell ref="L33:S33"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A5:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>